<commit_message>
Added Excel file reader class
</commit_message>
<xml_diff>
--- a/src/test/java/Utility/Inputs.xlsx
+++ b/src/test/java/Utility/Inputs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saudivtsa-my.sharepoint.com/personal/motaibi_saudivts_com/Documents/Desktop/Selenium/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MajedSultanAlotaibi\git\NUSUK-pre\src\test\java\Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{51A859E4-475E-4E5A-9FC8-4B0648C790CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B240CB-BBEE-4C31-8D21-8475329CD813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="11">
-  <si>
-    <t>Username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>Password</t>
   </si>
@@ -56,9 +53,6 @@
     <t>Confirm_password</t>
   </si>
   <si>
-    <t>USER11</t>
-  </si>
-  <si>
     <t>PAS111</t>
   </si>
   <si>
@@ -66,6 +60,24 @@
   </si>
   <si>
     <t>MAJED</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>EEEE</t>
+  </si>
+  <si>
+    <t>FFFF</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Hs622!@ad</t>
   </si>
 </sst>
 </file>
@@ -129,10 +141,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,79 +440,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>535352885</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -515,42 +516,36 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>535352885</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>535352885</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -561,42 +556,36 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6">
+        <v>535352885</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>535352885</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
@@ -607,39 +596,35 @@
       <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8">
+        <v>535352885</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>535352885</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{835FD481-8A9A-4AD5-AAAD-10C02ADBDD7A}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{231E5729-8E99-4C7A-B870-830B9DD3A804}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{C5DC61CD-F76B-41C9-A570-7F3AFBCB80B1}"/>
+    <hyperlink ref="C2" r:id="rId1" display="DUMMY@EMAIL" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{835FD481-8A9A-4AD5-AAAD-10C02ADBDD7A}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{231E5729-8E99-4C7A-B870-830B9DD3A804}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{C5DC61CD-F76B-41C9-A570-7F3AFBCB80B1}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{13CEC1F0-ED5A-4738-BDC8-4A6AAA818308}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{65510A8F-1728-4C97-8E98-E783E28CBF57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>